<commit_message>
2016-05-17掠夺(防御-秦字-杭州-白龙瀑分舵) YY List Update & Compare.xlsx Fixed
</commit_message>
<xml_diff>
--- a/5.16-5.22.xlsx
+++ b/5.16-5.22.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="164">
   <si>
     <t>ID</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Test</t>
   </si>
   <si>
-    <t>TEST</t>
-  </si>
-  <si>
     <t>KILL</t>
   </si>
   <si>
@@ -443,6 +440,90 @@
   </si>
   <si>
     <t>临风望月爱啪啪</t>
+  </si>
+  <si>
+    <t>机智勇敢的小免</t>
+  </si>
+  <si>
+    <t>池小晩</t>
+  </si>
+  <si>
+    <t>诸天花雨</t>
+  </si>
+  <si>
+    <t>南宫絮语</t>
+  </si>
+  <si>
+    <t>吕小栋</t>
+  </si>
+  <si>
+    <t>浪迹小秦</t>
+  </si>
+  <si>
+    <t>花兮兮兮兮</t>
+  </si>
+  <si>
+    <t>灬醉丨雲嫣</t>
+  </si>
+  <si>
+    <t>万心忧</t>
+  </si>
+  <si>
+    <t>何月凡</t>
+  </si>
+  <si>
+    <t>丶初馨</t>
+  </si>
+  <si>
+    <t>亲爱的未闻花名</t>
+  </si>
+  <si>
+    <t>蚩尤魔人</t>
+  </si>
+  <si>
+    <t>东风路三狗蛋</t>
+  </si>
+  <si>
+    <t>风暖伤</t>
+  </si>
+  <si>
+    <t>其实想玩刀客</t>
+  </si>
+  <si>
+    <t>紫舞流年</t>
+  </si>
+  <si>
+    <t>青城爱未恋</t>
+  </si>
+  <si>
+    <t>青羽墨染云</t>
+  </si>
+  <si>
+    <t>追风少年鹰老七</t>
+  </si>
+  <si>
+    <t>小阿鏡</t>
+  </si>
+  <si>
+    <t>绫月薇</t>
+  </si>
+  <si>
+    <t>一直梨花压海棠</t>
+  </si>
+  <si>
+    <t>牛奶奶奶奶</t>
+  </si>
+  <si>
+    <t>树儿高高长</t>
+  </si>
+  <si>
+    <t>格七</t>
+  </si>
+  <si>
+    <t>格殺</t>
+  </si>
+  <si>
+    <t>再见是否红着脸</t>
   </si>
 </sst>
 </file>
@@ -516,14 +597,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -809,41 +890,42 @@
   <dimension ref="A1:S110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="I1" s="7" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="M1" s="7" t="s">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="M1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="Q1" s="7" t="s">
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="Q1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -893,14 +975,17 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="9">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -908,7 +993,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -916,7 +1007,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -924,7 +1021,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -932,7 +1035,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -940,7 +1049,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6</v>
+      </c>
+      <c r="F8" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -948,7 +1063,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="E9" s="1">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -956,7 +1077,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="E10" s="1">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -964,7 +1091,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="E11" s="1">
+        <v>9</v>
+      </c>
+      <c r="F11" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -972,7 +1105,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="E12" s="1">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -980,7 +1119,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="E13" s="1">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -988,7 +1133,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="E14" s="1">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -996,7 +1147,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="E15" s="1">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1004,647 +1161,1061 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="E16" s="1">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="E17" s="1">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="E18" s="1">
+        <v>16</v>
+      </c>
+      <c r="F18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="E19" s="1">
+        <v>17</v>
+      </c>
+      <c r="F19" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="E20" s="1">
+        <v>18</v>
+      </c>
+      <c r="F20" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="E21" s="1">
+        <v>19</v>
+      </c>
+      <c r="F21" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="E22" s="1">
+        <v>20</v>
+      </c>
+      <c r="F22" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="E23" s="1">
+        <v>21</v>
+      </c>
+      <c r="F23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="E24" s="1">
+        <v>22</v>
+      </c>
+      <c r="F24" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="E25" s="1">
+        <v>23</v>
+      </c>
+      <c r="F25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="E26" s="1">
+        <v>24</v>
+      </c>
+      <c r="F26" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="E27" s="1">
+        <v>25</v>
+      </c>
+      <c r="F27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="E28" s="1">
+        <v>26</v>
+      </c>
+      <c r="F28" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+      <c r="E29" s="1">
+        <v>27</v>
+      </c>
+      <c r="F29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="E30" s="1">
+        <v>28</v>
+      </c>
+      <c r="F30" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="E31" s="1">
+        <v>29</v>
+      </c>
+      <c r="F31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="E32" s="1">
+        <v>30</v>
+      </c>
+      <c r="F32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="E33" s="1">
+        <v>31</v>
+      </c>
+      <c r="F33" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="E34" s="1">
+        <v>32</v>
+      </c>
+      <c r="F34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+      <c r="E35" s="1">
+        <v>33</v>
+      </c>
+      <c r="F35" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="E36" s="1">
+        <v>34</v>
+      </c>
+      <c r="F36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="E37" s="1">
+        <v>35</v>
+      </c>
+      <c r="F37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E38" s="1">
+        <v>36</v>
+      </c>
+      <c r="F38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="E39" s="1">
+        <v>37</v>
+      </c>
+      <c r="F39" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="E40" s="1">
+        <v>38</v>
+      </c>
+      <c r="F40" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="E41" s="1">
+        <v>39</v>
+      </c>
+      <c r="F41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="E42" s="1">
+        <v>40</v>
+      </c>
+      <c r="F42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="E43" s="1">
+        <v>41</v>
+      </c>
+      <c r="F43" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="E44" s="1">
+        <v>42</v>
+      </c>
+      <c r="F44" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+      <c r="E45" s="1">
+        <v>43</v>
+      </c>
+      <c r="F45" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="E46" s="1">
+        <v>44</v>
+      </c>
+      <c r="F46" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+      <c r="E47" s="1">
+        <v>45</v>
+      </c>
+      <c r="F47" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="E48" s="1">
+        <v>46</v>
+      </c>
+      <c r="F48" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="E49" s="1">
+        <v>47</v>
+      </c>
+      <c r="F49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="E50" s="1">
+        <v>48</v>
+      </c>
+      <c r="F50" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="E51" s="1">
+        <v>49</v>
+      </c>
+      <c r="F51" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="E52" s="1">
+        <v>50</v>
+      </c>
+      <c r="F52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="E53" s="1">
+        <v>51</v>
+      </c>
+      <c r="F53" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+      <c r="E54" s="1">
+        <v>52</v>
+      </c>
+      <c r="F54" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="E55" s="1">
+        <v>53</v>
+      </c>
+      <c r="F55" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="E56" s="1">
+        <v>54</v>
+      </c>
+      <c r="F56" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="E57" s="1">
+        <v>55</v>
+      </c>
+      <c r="F57" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+      <c r="E58" s="1">
+        <v>56</v>
+      </c>
+      <c r="F58" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="E59" s="1">
+        <v>57</v>
+      </c>
+      <c r="F59" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="E60" s="1">
+        <v>58</v>
+      </c>
+      <c r="F60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="E61" s="1">
+        <v>59</v>
+      </c>
+      <c r="F61" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="E62" s="1">
+        <v>60</v>
+      </c>
+      <c r="F62" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="E63" s="1">
+        <v>61</v>
+      </c>
+      <c r="F63" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="E64" s="1">
+        <v>62</v>
+      </c>
+      <c r="F64" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+      <c r="E65" s="1">
+        <v>63</v>
+      </c>
+      <c r="F65" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="E66" s="1">
+        <v>64</v>
+      </c>
+      <c r="F66" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="E67" s="1">
+        <v>65</v>
+      </c>
+      <c r="F67" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="E68" s="1">
+        <v>66</v>
+      </c>
+      <c r="F68" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="E69" s="1">
+        <v>67</v>
+      </c>
+      <c r="F69" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="E70" s="1">
+        <v>68</v>
+      </c>
+      <c r="F70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="E71" s="1">
+        <v>69</v>
+      </c>
+      <c r="F71" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="E72" s="1">
+        <v>70</v>
+      </c>
+      <c r="F72" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="E73" s="1">
+        <v>71</v>
+      </c>
+      <c r="F73" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="E74" s="1">
+        <v>72</v>
+      </c>
+      <c r="F74" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="E75" s="1">
+        <v>73</v>
+      </c>
+      <c r="F75" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="E76" s="1">
+        <v>74</v>
+      </c>
+      <c r="F76" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="E77" s="1">
+        <v>75</v>
+      </c>
+      <c r="F77" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="E78" s="1">
+        <v>76</v>
+      </c>
+      <c r="F78" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="E79" s="1">
+        <v>77</v>
+      </c>
+      <c r="F79" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="E80" s="1">
+        <v>78</v>
+      </c>
+      <c r="F80" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="E81" s="1">
+        <v>79</v>
+      </c>
+      <c r="F81" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="E82" s="1">
+        <v>80</v>
+      </c>
+      <c r="F82" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="E83" s="1">
+        <v>81</v>
+      </c>
+      <c r="F83" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="E84" s="1">
+        <v>82</v>
+      </c>
+      <c r="F84" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -1652,7 +2223,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -1660,7 +2231,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -1668,7 +2239,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -1676,7 +2247,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -1684,7 +2255,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -1692,7 +2263,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -1700,7 +2271,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -1708,7 +2279,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -1716,7 +2287,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -1724,7 +2295,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -1732,7 +2303,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -1740,7 +2311,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -1748,7 +2319,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -1756,7 +2327,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1816,85 +2387,85 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="I1" s="7" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="M1" s="7" t="s">
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="M1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
+      <c r="A2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1947,13 +2518,13 @@
         <v>19</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
@@ -1962,7 +2533,7 @@
       </c>
       <c r="B2" s="5">
         <f>COUNTIF(掠夺总榜!A$1:S$150,$A2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTIF(盟会战!A$1:Q$150,$A2)</f>
@@ -1973,7 +2544,7 @@
       </c>
       <c r="E2" s="3">
         <f>SUM(B2,C2,D2)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G2" s="3">
         <f>IF($E2&gt;6,6,$E2)</f>
@@ -1985,7 +2556,7 @@
       </c>
       <c r="J2" s="3">
         <f>SUM(E2:E140)-I2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2031,13 +2602,13 @@
         <v>19</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
@@ -2046,7 +2617,7 @@
       </c>
       <c r="B2" s="5">
         <f>COUNTIF(掠夺总榜!A$1:S$150,$A2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTIF(盟会战!A$1:Q$150,$A2)</f>
@@ -2057,7 +2628,7 @@
       </c>
       <c r="E2" s="3">
         <f>SUM(B2,C2,D2)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3">
@@ -2070,7 +2641,7 @@
       </c>
       <c r="J2" s="3">
         <f>SUM(E2:E150)-I2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2116,14 +2687,14 @@
         <v>19</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H1" s="3"/>
       <c r="I1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
@@ -2135,7 +2706,7 @@
       </c>
       <c r="B2" s="5">
         <f>COUNTIF(掠夺总榜!A$1:S$150,$A2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTIF(盟会战!A$1:Q$150,$A2)</f>
@@ -2146,7 +2717,7 @@
       </c>
       <c r="E2" s="3">
         <f>SUM(B2,C2,D2)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="3">
@@ -2160,7 +2731,7 @@
       </c>
       <c r="J2" s="3">
         <f>SUM(E2:E150)-I2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -2212,13 +2783,13 @@
         <v>19</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
@@ -2227,7 +2798,7 @@
       </c>
       <c r="B2" s="5">
         <f>COUNTIF(掠夺总榜!A$1:S$150,$A2)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="3">
         <f>COUNTIF(盟会战!A$1:Q$150,$A2)</f>
@@ -2238,7 +2809,7 @@
       </c>
       <c r="E2" s="3">
         <f>SUM(B2,C2,D2)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G2" s="3">
         <f>IF($E2&gt;6,6,$E2)</f>
@@ -2250,7 +2821,7 @@
       </c>
       <c r="J2" s="3">
         <f>SUM(E2:E150)-I2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2282,7 +2853,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Some Update  & Redundancy Removed
</commit_message>
<xml_diff>
--- a/5.16-5.22.xlsx
+++ b/5.16-5.22.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="掠夺总榜" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="190">
   <si>
     <t>ID</t>
   </si>
@@ -115,9 +115,6 @@
     <t>帮派溢出箱子</t>
   </si>
   <si>
-    <t>2016-04-04-狗</t>
-  </si>
-  <si>
     <t>椛灯</t>
   </si>
   <si>
@@ -524,6 +521,87 @@
   </si>
   <si>
     <t>再见是否红着脸</t>
+  </si>
+  <si>
+    <t>＊下水道的白</t>
+  </si>
+  <si>
+    <t>万宥茚黧</t>
+  </si>
+  <si>
+    <t>FateLibra</t>
+  </si>
+  <si>
+    <t>假老练</t>
+  </si>
+  <si>
+    <t>FateScorpio</t>
+  </si>
+  <si>
+    <t>娇软の小屁股</t>
+  </si>
+  <si>
+    <t>友善的咸鱼白</t>
+  </si>
+  <si>
+    <t>巡山的人</t>
+  </si>
+  <si>
+    <t>可爱琳</t>
+  </si>
+  <si>
+    <t>我是天香的啊</t>
+  </si>
+  <si>
+    <t>叶菡</t>
+  </si>
+  <si>
+    <t>池小晚</t>
+  </si>
+  <si>
+    <t>帅气无敌康爸爸</t>
+  </si>
+  <si>
+    <t>安好晴天</t>
+  </si>
+  <si>
+    <t>毕夏有毓</t>
+  </si>
+  <si>
+    <t>涛声依旧彡</t>
+  </si>
+  <si>
+    <t>流浪的小花狼</t>
+  </si>
+  <si>
+    <t>离殇天丶</t>
+  </si>
+  <si>
+    <t>秦友善。</t>
+  </si>
+  <si>
+    <t>纯洁友善的殇</t>
+  </si>
+  <si>
+    <t>男人应有的自豪</t>
+  </si>
+  <si>
+    <t>胡大力</t>
+  </si>
+  <si>
+    <t>颓废老男人</t>
+  </si>
+  <si>
+    <t>轻素剪云端</t>
+  </si>
+  <si>
+    <t>陌路莫回</t>
+  </si>
+  <si>
+    <t>青骢绝骑塑天荒</t>
+  </si>
+  <si>
+    <t>2016-05-16-轩</t>
   </si>
 </sst>
 </file>
@@ -579,7 +657,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -605,6 +683,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -887,10 +971,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,13 +1064,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="7">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -993,13 +1078,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -1007,13 +1092,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -1021,13 +1106,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="1">
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1035,13 +1120,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="1">
         <v>5</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1049,13 +1134,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="1">
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1063,13 +1148,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="1">
         <v>7</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1077,13 +1162,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E10" s="1">
         <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1091,13 +1176,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E11" s="1">
         <v>9</v>
       </c>
       <c r="F11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1105,13 +1190,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E12" s="1">
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1119,13 +1204,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" s="1">
         <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1133,13 +1218,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14" s="1">
         <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1147,13 +1232,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15" s="1">
         <v>13</v>
       </c>
       <c r="F15" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1161,13 +1246,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16" s="1">
         <v>14</v>
       </c>
       <c r="F16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1175,13 +1260,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17" s="1">
         <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1189,13 +1274,13 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E18" s="1">
         <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1203,13 +1288,13 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E19" s="1">
         <v>17</v>
       </c>
       <c r="F19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1217,13 +1302,13 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E20" s="1">
         <v>18</v>
       </c>
       <c r="F20" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1231,13 +1316,13 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" s="1">
         <v>19</v>
       </c>
       <c r="F21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1245,13 +1330,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="1">
         <v>20</v>
       </c>
       <c r="F22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1259,13 +1344,13 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E23" s="1">
         <v>21</v>
       </c>
       <c r="F23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1273,13 +1358,13 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E24" s="1">
         <v>22</v>
       </c>
       <c r="F24" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1287,13 +1372,13 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E25" s="1">
         <v>23</v>
       </c>
       <c r="F25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1301,13 +1386,13 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E26" s="1">
         <v>24</v>
       </c>
       <c r="F26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1315,13 +1400,13 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E27" s="1">
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1329,13 +1414,13 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E28" s="1">
         <v>26</v>
       </c>
       <c r="F28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1343,13 +1428,13 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E29" s="1">
         <v>27</v>
       </c>
       <c r="F29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1357,13 +1442,13 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E30" s="1">
         <v>28</v>
       </c>
       <c r="F30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1371,13 +1456,13 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E31" s="1">
         <v>29</v>
       </c>
       <c r="F31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1385,13 +1470,13 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E32" s="1">
         <v>30</v>
       </c>
       <c r="F32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1399,13 +1484,13 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E33" s="1">
         <v>31</v>
       </c>
       <c r="F33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1413,13 +1498,13 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E34" s="1">
         <v>32</v>
       </c>
       <c r="F34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1427,13 +1512,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E35" s="1">
         <v>33</v>
       </c>
       <c r="F35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1441,13 +1526,13 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E36" s="1">
         <v>34</v>
       </c>
       <c r="F36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1455,13 +1540,13 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E37" s="1">
         <v>35</v>
       </c>
       <c r="F37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1469,13 +1554,13 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E38" s="1">
         <v>36</v>
       </c>
       <c r="F38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1483,13 +1568,13 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E39" s="1">
         <v>37</v>
       </c>
       <c r="F39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1497,13 +1582,13 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E40" s="1">
         <v>38</v>
       </c>
       <c r="F40" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1511,13 +1596,13 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E41" s="1">
         <v>39</v>
       </c>
       <c r="F41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1525,13 +1610,13 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E42" s="1">
         <v>40</v>
       </c>
       <c r="F42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1539,13 +1624,13 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E43" s="1">
         <v>41</v>
       </c>
       <c r="F43" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1553,13 +1638,13 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E44" s="1">
         <v>42</v>
       </c>
       <c r="F44" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1567,13 +1652,13 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E45" s="1">
         <v>43</v>
       </c>
       <c r="F45" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1581,13 +1666,13 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E46" s="1">
         <v>44</v>
       </c>
       <c r="F46" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1595,13 +1680,13 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E47" s="1">
         <v>45</v>
       </c>
       <c r="F47" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1609,13 +1694,13 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E48" s="1">
         <v>46</v>
       </c>
       <c r="F48" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1623,13 +1708,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E49" s="1">
         <v>47</v>
       </c>
       <c r="F49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1637,13 +1722,13 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E50" s="1">
         <v>48</v>
       </c>
       <c r="F50" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1651,13 +1736,13 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E51" s="1">
         <v>49</v>
       </c>
       <c r="F51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1665,13 +1750,13 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E52" s="1">
         <v>50</v>
       </c>
       <c r="F52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1679,13 +1764,13 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E53" s="1">
         <v>51</v>
       </c>
       <c r="F53" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1693,13 +1778,13 @@
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E54" s="1">
         <v>52</v>
       </c>
       <c r="F54" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1707,13 +1792,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E55" s="1">
         <v>53</v>
       </c>
       <c r="F55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1721,13 +1806,13 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E56" s="1">
         <v>54</v>
       </c>
       <c r="F56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1735,13 +1820,13 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E57" s="1">
         <v>55</v>
       </c>
       <c r="F57" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1749,13 +1834,13 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E58" s="1">
         <v>56</v>
       </c>
       <c r="F58" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1763,13 +1848,13 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E59" s="1">
         <v>57</v>
       </c>
       <c r="F59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -1777,13 +1862,13 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E60" s="1">
         <v>58</v>
       </c>
       <c r="F60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -1791,13 +1876,13 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E61" s="1">
         <v>59</v>
       </c>
       <c r="F61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -1805,13 +1890,13 @@
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E62" s="1">
         <v>60</v>
       </c>
       <c r="F62" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -1819,13 +1904,13 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E63" s="1">
         <v>61</v>
       </c>
       <c r="F63" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1833,13 +1918,13 @@
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E64" s="1">
         <v>62</v>
       </c>
       <c r="F64" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1847,13 +1932,13 @@
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E65" s="1">
         <v>63</v>
       </c>
       <c r="F65" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1861,13 +1946,13 @@
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E66" s="1">
         <v>64</v>
       </c>
       <c r="F66" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1875,13 +1960,13 @@
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E67" s="1">
         <v>65</v>
       </c>
       <c r="F67" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1889,13 +1974,13 @@
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E68" s="1">
         <v>66</v>
       </c>
       <c r="F68" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1903,13 +1988,13 @@
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E69" s="1">
         <v>67</v>
       </c>
       <c r="F69" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1917,13 +2002,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E70" s="1">
         <v>68</v>
       </c>
       <c r="F70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -1931,13 +2016,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E71" s="1">
         <v>69</v>
       </c>
       <c r="F71" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -1945,13 +2030,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E72" s="1">
         <v>70</v>
       </c>
       <c r="F72" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -1959,13 +2044,13 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E73" s="1">
         <v>71</v>
       </c>
       <c r="F73" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -1973,13 +2058,13 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E74" s="1">
         <v>72</v>
       </c>
       <c r="F74" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -1987,13 +2072,13 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E75" s="1">
         <v>73</v>
       </c>
       <c r="F75" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2001,13 +2086,13 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E76" s="1">
         <v>74</v>
       </c>
       <c r="F76" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2015,13 +2100,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E77" s="1">
         <v>75</v>
       </c>
       <c r="F77" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2029,13 +2114,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E78" s="1">
         <v>76</v>
       </c>
       <c r="F78" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2043,13 +2128,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E79" s="1">
         <v>77</v>
       </c>
       <c r="F79" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2057,13 +2142,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E80" s="1">
         <v>78</v>
       </c>
       <c r="F80" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2071,13 +2156,13 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E81" s="1">
         <v>79</v>
       </c>
       <c r="F81" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2085,13 +2170,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E82" s="1">
         <v>80</v>
       </c>
       <c r="F82" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2099,13 +2184,13 @@
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E83" s="1">
         <v>81</v>
       </c>
       <c r="F83" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2113,13 +2198,13 @@
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E84" s="1">
         <v>82</v>
       </c>
       <c r="F84" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2127,7 +2212,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2135,7 +2220,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2143,7 +2228,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2151,7 +2236,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2159,7 +2244,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2167,7 +2252,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2175,7 +2260,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2183,7 +2268,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2191,7 +2276,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2199,7 +2284,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2207,7 +2292,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2215,7 +2300,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -2223,7 +2308,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -2231,7 +2316,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -2239,7 +2324,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2247,7 +2332,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -2255,7 +2340,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -2263,7 +2348,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2271,7 +2356,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2279,7 +2364,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -2287,7 +2372,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2295,7 +2380,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -2303,7 +2388,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -2311,7 +2396,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -2319,7 +2404,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -2327,7 +2412,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2345,10 +2430,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2378,13 +2464,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
@@ -2410,7 +2503,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>27</v>
+        <v>189</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -2468,6 +2561,1046 @@
         <v>22</v>
       </c>
     </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>81</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F4" s="1">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1">
+        <v>42</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J4" s="1">
+        <v>5</v>
+      </c>
+      <c r="K4" s="1">
+        <v>62</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N4" s="1">
+        <v>13</v>
+      </c>
+      <c r="O4" s="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>44</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>10</v>
+      </c>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="N5" s="11">
+        <v>5</v>
+      </c>
+      <c r="O5" s="11">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>51</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J6" s="1">
+        <v>3</v>
+      </c>
+      <c r="K6" s="1">
+        <v>21</v>
+      </c>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="N6" s="11">
+        <v>1</v>
+      </c>
+      <c r="O6" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>57</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="J7" s="1">
+        <v>16</v>
+      </c>
+      <c r="K7" s="1">
+        <v>114</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="N7" s="1">
+        <v>13</v>
+      </c>
+      <c r="O7" s="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" s="11">
+        <v>13</v>
+      </c>
+      <c r="C8" s="11">
+        <v>97</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="1">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1">
+        <v>63</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J8" s="11">
+        <v>11</v>
+      </c>
+      <c r="K8" s="11">
+        <v>111</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N8" s="11">
+        <v>6</v>
+      </c>
+      <c r="O8" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>11</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J9" s="11">
+        <v>7</v>
+      </c>
+      <c r="K9" s="11">
+        <v>23</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="N9" s="1">
+        <v>5</v>
+      </c>
+      <c r="O9" s="1">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B10" s="1">
+        <v>5</v>
+      </c>
+      <c r="C10" s="1">
+        <v>62</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="11">
+        <v>15</v>
+      </c>
+      <c r="G10" s="11">
+        <v>121</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>6</v>
+      </c>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="N10" s="1">
+        <v>1</v>
+      </c>
+      <c r="O10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>18</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="1">
+        <v>27</v>
+      </c>
+      <c r="G11" s="1">
+        <v>107</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="J11" s="1">
+        <v>2</v>
+      </c>
+      <c r="K11" s="1">
+        <v>15</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N11" s="11">
+        <v>10</v>
+      </c>
+      <c r="O11" s="11">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="1">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1">
+        <v>51</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="1">
+        <v>13</v>
+      </c>
+      <c r="G12" s="1">
+        <v>101</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="1">
+        <v>6</v>
+      </c>
+      <c r="K12" s="1">
+        <v>61</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" s="1">
+        <v>11</v>
+      </c>
+      <c r="O12" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F13" s="1">
+        <v>6</v>
+      </c>
+      <c r="G13" s="1">
+        <v>79</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" s="11">
+        <v>0</v>
+      </c>
+      <c r="K13" s="11">
+        <v>15</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N13" s="1">
+        <v>17</v>
+      </c>
+      <c r="O13" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B14" s="1">
+        <v>5</v>
+      </c>
+      <c r="C14" s="1">
+        <v>15</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J14" s="11">
+        <v>0</v>
+      </c>
+      <c r="K14" s="11">
+        <v>12</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="N14" s="1">
+        <v>5</v>
+      </c>
+      <c r="O14" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B15" s="1">
+        <v>3</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F15" s="1">
+        <v>1</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J15" s="1">
+        <v>22</v>
+      </c>
+      <c r="K15" s="1">
+        <v>165</v>
+      </c>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="N15" s="11">
+        <v>3</v>
+      </c>
+      <c r="O15" s="11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B16" s="1">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1">
+        <v>23</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0</v>
+      </c>
+      <c r="G16" s="11">
+        <v>3</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="11">
+        <v>12</v>
+      </c>
+      <c r="K16" s="11">
+        <v>74</v>
+      </c>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N16" s="1">
+        <v>0</v>
+      </c>
+      <c r="O16" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17" s="11">
+        <v>15</v>
+      </c>
+      <c r="C17" s="11">
+        <v>53</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="11">
+        <v>1</v>
+      </c>
+      <c r="G17" s="11">
+        <v>26</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J17" s="11">
+        <v>12</v>
+      </c>
+      <c r="K17" s="11">
+        <v>101</v>
+      </c>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N17" s="11">
+        <v>7</v>
+      </c>
+      <c r="O17" s="11">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" s="1">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1">
+        <v>27</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>40</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="11">
+        <v>1</v>
+      </c>
+      <c r="K18" s="11">
+        <v>18</v>
+      </c>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="N18" s="11">
+        <v>3</v>
+      </c>
+      <c r="O18" s="11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" s="1">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1">
+        <v>14</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F19" s="1">
+        <v>9</v>
+      </c>
+      <c r="G19" s="1">
+        <v>67</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J19" s="1">
+        <v>4</v>
+      </c>
+      <c r="K19" s="1">
+        <v>7</v>
+      </c>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="N19" s="1">
+        <v>2</v>
+      </c>
+      <c r="O19" s="1">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B20" s="1">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1">
+        <v>18</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F20" s="1">
+        <v>97</v>
+      </c>
+      <c r="G20" s="1">
+        <v>780</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J20" s="1">
+        <v>16</v>
+      </c>
+      <c r="K20" s="1">
+        <v>99</v>
+      </c>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="N20" s="1">
+        <v>3</v>
+      </c>
+      <c r="O20" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="1">
+        <v>11</v>
+      </c>
+      <c r="C21" s="1">
+        <v>90</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J21" s="1">
+        <v>4</v>
+      </c>
+      <c r="K21" s="1">
+        <v>36</v>
+      </c>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="N21" s="11">
+        <v>5</v>
+      </c>
+      <c r="O21" s="11">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" s="1">
+        <v>26</v>
+      </c>
+      <c r="C22" s="1">
+        <v>94</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J22" s="1">
+        <v>19</v>
+      </c>
+      <c r="K22" s="1">
+        <v>184</v>
+      </c>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="N22" s="11">
+        <v>3</v>
+      </c>
+      <c r="O22" s="11">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2</v>
+      </c>
+      <c r="C23" s="1">
+        <v>41</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="J23" s="1">
+        <v>6</v>
+      </c>
+      <c r="K23" s="1">
+        <v>63</v>
+      </c>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="N23" s="1">
+        <v>8</v>
+      </c>
+      <c r="O23" s="1">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="1">
+        <v>7</v>
+      </c>
+      <c r="C24" s="1">
+        <v>64</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <v>5</v>
+      </c>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="N24" s="1">
+        <v>21</v>
+      </c>
+      <c r="O24" s="1">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B25" s="1">
+        <v>7</v>
+      </c>
+      <c r="C25" s="1">
+        <v>27</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" s="1">
+        <v>7</v>
+      </c>
+      <c r="K25" s="1">
+        <v>11</v>
+      </c>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N25" s="11">
+        <v>4</v>
+      </c>
+      <c r="O25" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1">
+        <v>135</v>
+      </c>
+      <c r="C26" s="1">
+        <v>888</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" s="1">
+        <v>9</v>
+      </c>
+      <c r="K26" s="1">
+        <v>50</v>
+      </c>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="N26" s="11">
+        <v>3</v>
+      </c>
+      <c r="O26" s="11">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="J27" s="1">
+        <v>14</v>
+      </c>
+      <c r="K27" s="1">
+        <v>42</v>
+      </c>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="N27" s="11">
+        <v>5</v>
+      </c>
+      <c r="O27" s="11">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J28" s="1">
+        <v>14</v>
+      </c>
+      <c r="K28" s="1">
+        <v>65</v>
+      </c>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N28" s="11">
+        <v>4</v>
+      </c>
+      <c r="O28" s="11">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="J29" s="11">
+        <v>1</v>
+      </c>
+      <c r="K29" s="11">
+        <v>8</v>
+      </c>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N29" s="11">
+        <v>158</v>
+      </c>
+      <c r="O29" s="11">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J30" s="11">
+        <v>9</v>
+      </c>
+      <c r="K30" s="11">
+        <v>56</v>
+      </c>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="11"/>
+      <c r="C31" s="11"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J31" s="1">
+        <v>200</v>
+      </c>
+      <c r="K31" s="1">
+        <v>1434</v>
+      </c>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:C1"/>
@@ -2482,14 +3615,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="4" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -2499,7 +3634,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -2528,7 +3663,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="5">
@@ -2566,14 +3701,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
@@ -2583,7 +3720,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -2612,7 +3749,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="5">
@@ -2651,14 +3788,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.28515625" bestFit="1" customWidth="1"/>
@@ -2668,7 +3807,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -2701,7 +3840,7 @@
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="5">
@@ -2744,15 +3883,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="4" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -2764,7 +3904,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -2793,7 +3933,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="5">
@@ -2831,9 +3971,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>

</xml_diff>